<commit_message>
l26 600 qpsk wip
</commit_message>
<xml_diff>
--- a/600_iir_llpf_calc.xlsx
+++ b/600_iir_llpf_calc.xlsx
@@ -478,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -489,7 +489,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -640,7 +640,7 @@
         <v>25</v>
       </c>
       <c r="B16" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -666,7 +666,7 @@
       </c>
       <c r="B20" s="2">
         <f>ROUND(B19*B13*B16,0)</f>
-        <v>2829</v>
+        <v>707</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
@@ -678,7 +678,7 @@
       </c>
       <c r="B21" s="2">
         <f>ROUND(B19*B14*B16,0)</f>
-        <v>2829</v>
+        <v>707</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
@@ -709,7 +709,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -866,7 +866,7 @@
         <v>25</v>
       </c>
       <c r="B18" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -892,7 +892,7 @@
       </c>
       <c r="B22" s="2">
         <f>ROUND(B21*B13*B18,0)</f>
-        <v>2016</v>
+        <v>8062</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
@@ -904,7 +904,7 @@
       </c>
       <c r="B23" s="2">
         <f>ROUND(B21*B14*B18,0)</f>
-        <v>2016</v>
+        <v>8062</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
qpsk 600 l26 tuning
</commit_message>
<xml_diff>
--- a/600_iir_llpf_calc.xlsx
+++ b/600_iir_llpf_calc.xlsx
@@ -478,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -489,7 +489,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -640,7 +640,7 @@
         <v>25</v>
       </c>
       <c r="B16" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -666,7 +666,7 @@
       </c>
       <c r="B20" s="2">
         <f>ROUND(B19*B13*B16,0)</f>
-        <v>707</v>
+        <v>1414</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
@@ -678,7 +678,7 @@
       </c>
       <c r="B21" s="2">
         <f>ROUND(B19*B14*B16,0)</f>
-        <v>707</v>
+        <v>1414</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
qpsk 600 l26 revert to previous best
</commit_message>
<xml_diff>
--- a/600_iir_llpf_calc.xlsx
+++ b/600_iir_llpf_calc.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AC589E-0E74-F44B-A9A5-7512DF266937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15225" yWindow="120" windowWidth="13575" windowHeight="17880"/>
+    <workbookView xWindow="15220" yWindow="120" windowWidth="13580" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoopFilter LPF" sheetId="4" r:id="rId1"/>
     <sheet name="Branch LPF" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -117,8 +123,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -162,9 +168,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -478,56 +483,56 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>14400</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -539,7 +544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -554,7 +559,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -569,7 +574,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -581,7 +586,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -590,7 +595,7 @@
         <v>2.0218174810193945</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -599,7 +604,7 @@
         <v>1.9781825189806053</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -611,7 +616,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -623,7 +628,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -635,15 +640,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="B16" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -651,7 +656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -660,35 +665,35 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <f>ROUND(B19*B13*B16,0)</f>
-        <v>1414</v>
+        <v>2829</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <f>ROUND(B19*B14*B16,0)</f>
-        <v>1414</v>
+        <v>2829</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <f>ROUND(B19*B12,0)</f>
         <v>32061</v>
       </c>
@@ -705,49 +710,49 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>300</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>14400</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -759,7 +764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -774,7 +779,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -789,7 +794,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -801,7 +806,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -810,7 +815,7 @@
         <v>2.1310869256304765</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -819,7 +824,7 @@
         <v>1.8689130743695235</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -831,7 +836,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -843,7 +848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -855,21 +860,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -877,7 +882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -886,45 +891,41 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <f>ROUND(B21*B13*B18,0)</f>
-        <v>8062</v>
+        <v>2016</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <f>ROUND(B21*B14*B18,0)</f>
-        <v>8062</v>
+        <v>2016</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <f>ROUND(B21*B12,0)</f>
         <v>28737</v>
       </c>
       <c r="D24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
adjust qpsk 600 intermed decimation
</commit_message>
<xml_diff>
--- a/600_iir_llpf_calc.xlsx
+++ b/600_iir_llpf_calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC4A554-8D53-4645-9828-EEB0C34C5C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577F900B-29B3-864B-BC8E-AEC0233F6AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2180" yWindow="100" windowWidth="13580" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -515,7 +515,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -538,7 +538,7 @@
       </c>
       <c r="B4">
         <f>2*PI()*B2</f>
-        <v>314.15926535897933</v>
+        <v>157.07963267948966</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -565,7 +565,7 @@
       </c>
       <c r="B6">
         <f>(2*B3)*TAN(B4*B5/2)</f>
-        <v>314.17172667928406</v>
+        <v>157.0811902889225</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -580,7 +580,7 @@
       </c>
       <c r="B8">
         <f>B6*B5</f>
-        <v>2.1817481019394725E-2</v>
+        <v>1.0908415992286284E-2</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
@@ -592,7 +592,7 @@
       </c>
       <c r="B9">
         <f>2+(B8)</f>
-        <v>2.0218174810193945</v>
+        <v>2.0109084159922861</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -601,7 +601,7 @@
       </c>
       <c r="B10">
         <f>2-B8</f>
-        <v>1.9781825189806053</v>
+        <v>1.9890915840077137</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -610,7 +610,7 @@
       </c>
       <c r="B12">
         <f>B10/B9</f>
-        <v>0.97841795194253212</v>
+        <v>0.98915075803001851</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -622,7 +622,7 @@
       </c>
       <c r="B13">
         <f>B8/B9</f>
-        <v>1.0791024028733996E-2</v>
+        <v>5.4246209849907598E-3</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -634,7 +634,7 @@
       </c>
       <c r="B14">
         <f>B8/B9</f>
-        <v>1.0791024028733996E-2</v>
+        <v>5.4246209849907598E-3</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -671,7 +671,7 @@
       </c>
       <c r="B20" s="1">
         <f>ROUND(B19*B13*B16,0)</f>
-        <v>354</v>
+        <v>178</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
@@ -683,7 +683,7 @@
       </c>
       <c r="B21" s="1">
         <f>ROUND(B19*B14*B16,0)</f>
-        <v>354</v>
+        <v>178</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
@@ -695,7 +695,7 @@
       </c>
       <c r="B22" s="1">
         <f>ROUND(B19*B12,0)</f>
-        <v>32061</v>
+        <v>32412</v>
       </c>
       <c r="D22" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
pre 600 gain change
</commit_message>
<xml_diff>
--- a/600_iir_llpf_calc.xlsx
+++ b/600_iir_llpf_calc.xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577F900B-29B3-864B-BC8E-AEC0233F6AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="100" windowWidth="13580" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2175" yWindow="105" windowWidth="13575" windowHeight="17880"/>
   </bookViews>
   <sheets>
     <sheet name="LoopFilter LPF" sheetId="4" r:id="rId1"/>
     <sheet name="Branch LPF" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -123,8 +117,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -237,7 +231,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -289,7 +283,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -483,45 +477,45 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -532,19 +526,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <f>2*PI()*B2</f>
-        <v>157.07963267948966</v>
+        <v>314.15926535897933</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -559,13 +553,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <f>(2*B3)*TAN(B4*B5/2)</f>
-        <v>157.0811902889225</v>
+        <v>314.17172667928406</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -574,73 +568,73 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
         <f>B6*B5</f>
-        <v>1.0908415992286284E-2</v>
+        <v>2.1817481019394725E-2</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
         <f>2+(B8)</f>
-        <v>2.0109084159922861</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.0218174810193945</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
         <f>2-B8</f>
-        <v>1.9890915840077137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1.9781825189806053</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <f>B10/B9</f>
-        <v>0.98915075803001851</v>
+        <v>0.97841795194253212</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13">
         <f>B8/B9</f>
-        <v>5.4246209849907598E-3</v>
+        <v>1.0791024028733996E-2</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
         <f>B8/B9</f>
-        <v>5.4246209849907598E-3</v>
+        <v>1.0791024028733996E-2</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -648,7 +642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -656,7 +650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -665,37 +659,37 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="1">
         <f>ROUND(B19*B13*B16,0)</f>
-        <v>178</v>
+        <v>354</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <f>ROUND(B19*B14*B16,0)</f>
-        <v>178</v>
+        <v>354</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="1">
         <f>ROUND(B19*B12,0)</f>
-        <v>32412</v>
+        <v>32061</v>
       </c>
       <c r="D22" t="s">
         <v>20</v>
@@ -710,27 +704,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -741,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -752,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -764,7 +758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -779,7 +773,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -794,7 +788,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -806,7 +800,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -815,7 +809,7 @@
         <v>2.1310869256304765</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -824,7 +818,7 @@
         <v>1.8689130743695235</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -836,7 +830,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -848,7 +842,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -860,13 +854,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -874,7 +868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -882,7 +876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -891,7 +885,7 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -903,7 +897,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -915,7 +909,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
600 retune 100Hz loop filter
</commit_message>
<xml_diff>
--- a/600_iir_llpf_calc.xlsx
+++ b/600_iir_llpf_calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="105" windowWidth="13575" windowHeight="17880" activeTab="1"/>
+    <workbookView xWindow="2175" yWindow="105" windowWidth="13575" windowHeight="17880"/>
   </bookViews>
   <sheets>
     <sheet name="LoopFilter LPF" sheetId="4" r:id="rId1"/>
@@ -480,7 +480,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -512,7 +512,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -535,7 +535,7 @@
       </c>
       <c r="B4">
         <f>2*PI()*B2</f>
-        <v>314.15926535897933</v>
+        <v>628.31853071795865</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -562,7 +562,7 @@
       </c>
       <c r="B6">
         <f>(2*B3)*TAN(B4*B5/2)</f>
-        <v>314.17172667928406</v>
+        <v>628.41823551790492</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -577,7 +577,7 @@
       </c>
       <c r="B8">
         <f>B6*B5</f>
-        <v>2.1817481019394725E-2</v>
+        <v>4.3640155244298956E-2</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
@@ -589,7 +589,7 @@
       </c>
       <c r="B9">
         <f>2+(B8)</f>
-        <v>2.0218174810193945</v>
+        <v>2.0436401552442991</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -598,7 +598,7 @@
       </c>
       <c r="B10">
         <f>2-B8</f>
-        <v>1.9781825189806053</v>
+        <v>1.9563598447557011</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -607,7 +607,7 @@
       </c>
       <c r="B12">
         <f>B10/B9</f>
-        <v>0.97841795194253212</v>
+        <v>0.95729174225480784</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -619,7 +619,7 @@
       </c>
       <c r="B13">
         <f>B8/B9</f>
-        <v>1.0791024028733996E-2</v>
+        <v>2.1354128872596048E-2</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -631,7 +631,7 @@
       </c>
       <c r="B14">
         <f>B8/B9</f>
-        <v>1.0791024028733996E-2</v>
+        <v>2.1354128872596048E-2</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -668,7 +668,7 @@
       </c>
       <c r="B20" s="1">
         <f>ROUND(B19*B13*B16,0)</f>
-        <v>354</v>
+        <v>700</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
@@ -680,7 +680,7 @@
       </c>
       <c r="B21" s="1">
         <f>ROUND(B19*B14*B16,0)</f>
-        <v>354</v>
+        <v>700</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
@@ -692,7 +692,7 @@
       </c>
       <c r="B22" s="1">
         <f>ROUND(B19*B12,0)</f>
-        <v>32061</v>
+        <v>31369</v>
       </c>
       <c r="D22" t="s">
         <v>20</v>
@@ -704,7 +704,7 @@
       </c>
       <c r="B27">
         <f>ROUND(SQRT('Branch LPF'!B2*('Branch LPF'!B2-'LoopFilter LPF'!B2)),0)</f>
-        <v>274</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -719,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>